<commit_message>
update calculator UI to 3 tabs, simplify
</commit_message>
<xml_diff>
--- a/Location_data.xlsx
+++ b/Location_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryan.morse\Documents\Aquaculture\Shellfish permitting and ecosystem services\Shellfish Calculators\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryan.morse\Documents\GitHub\Calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
     <sheet name="MA" sheetId="4" r:id="rId6"/>
     <sheet name="ME" sheetId="5" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="159">
   <si>
     <t>Barr</t>
   </si>
@@ -504,6 +504,9 @@
   </si>
   <si>
     <t>Farm 3</t>
+  </si>
+  <si>
+    <t>st_abrv</t>
   </si>
 </sst>
 </file>
@@ -513,7 +516,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -555,6 +558,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -588,7 +598,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -603,6 +613,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -887,7 +899,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -906,30 +918,34 @@
     <col min="13" max="13" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>143</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>68</v>
+        <v>158</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="5" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -949,7 +965,7 @@
         <v>-73.590170999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -969,7 +985,7 @@
         <v>-75.126329999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -986,7 +1002,7 @@
         <v>-70.280918999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1006,7 +1022,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1023,7 +1039,7 @@
         <v>-70.644469999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1040,7 +1056,7 @@
         <v>-70.865882999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1058,7 +1074,7 @@
       </c>
       <c r="H8" s="12"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1076,7 +1092,7 @@
       </c>
       <c r="H9" s="12"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1094,7 +1110,7 @@
       </c>
       <c r="H10" s="12"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1112,7 +1128,7 @@
       </c>
       <c r="H11" s="12"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1132,7 +1148,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1150,7 +1166,7 @@
       </c>
       <c r="H13" s="12"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1168,7 +1184,7 @@
       </c>
       <c r="H14" s="12"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1185,7 +1201,7 @@
         <v>-70.156924000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>

</xml_diff>